<commit_message>
ASK-56 Proces review commands of benchmark tests (partly)
</commit_message>
<xml_diff>
--- a/benchmarktests/assembly.kernel.benchmark.tests.io.tests/test-data/Benchmartktest - voorbeeld - 83-1.xlsx
+++ b/benchmarktests/assembly.kernel.benchmark.tests.io.tests/test-data/Benchmartktest - voorbeeld - 83-1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\wbi-assemblage-rekenkern\benchmarktests\testdefinitions\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\wbi-assemblage-rekenkern\benchmarktests\assembly.kernel.benchmark.tests.io.tests\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{743CE90E-89D7-45E9-BA38-E07D8CA717E3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{818DE218-869A-4F25-B4AA-E6D22FF1ED0F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="653" activeTab="10" xr2:uid="{34AC3CB5-6C6A-4A77-BC52-5E824B97181F}"/>
+    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11385" tabRatio="653" firstSheet="2" activeTab="10" xr2:uid="{34AC3CB5-6C6A-4A77-BC52-5E824B97181F}"/>
   </bookViews>
   <sheets>
     <sheet name="Informatiepagina" sheetId="1" r:id="rId1"/>
@@ -1718,7 +1718,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C158833E-EC89-433E-95ED-60C9389E8606}">
   <dimension ref="B1:F21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A10" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
@@ -2274,8 +2274,8 @@
   </sheetPr>
   <dimension ref="B1:L558"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A520" workbookViewId="0">
+      <selection activeCell="B523" sqref="B523:L523"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -25201,48 +25201,17 @@
       </c>
     </row>
     <row r="523" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B523" s="8">
-        <v>20.5168</v>
-      </c>
-      <c r="C523" s="9">
-        <v>21.02</v>
-      </c>
-      <c r="D523" s="23" t="str">
-        <f t="shared" si="16"/>
-        <v>+II</v>
-      </c>
-      <c r="E523" s="23" t="str">
-        <f t="shared" si="17"/>
-        <v>+II</v>
-      </c>
-      <c r="F523" s="9" t="str">
-        <f t="array" ref="F523">INDEX(STPH!$O$11:$O$34,IFERROR(MATCH(MIN(IF(STPH!$D$11:$D$34&gt;AVERAGE(B523,C523),STPH!$D$11:$D$34)),STPH!$D$11:$D$34),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="G523" s="9" t="str">
-        <f t="array" ref="G523">INDEX(STBI!$O$11:$O$36,IFERROR(MATCH(MIN(IF(STBI!$D$11:$D$36&gt;AVERAGE(B523,C523),STBI!$D$11:$D$36)),STBI!$D$11:$D$36),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="H523" s="9" t="str">
-        <f t="array" ref="H523">INDEX(GEKB!$K$11:$K$30,IFERROR(MATCH(MIN(IF(GEKB!$D$11:$D$30&gt;AVERAGE(B523,C523),GEKB!$D$11:$D$30)),GEKB!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="I523" s="9" t="str">
-        <f t="array" ref="I523">INDEX(DA!$K$11:$K$30,IFERROR(MATCH(MIN(IF(DA!$D$11:$D$30&gt;AVERAGE(B523,C523),DA!$D$11:$D$30)),DA!$D$11:$D$30),1))</f>
-        <v>+III</v>
-      </c>
-      <c r="J523" s="9" t="str">
-        <f t="array" ref="J523">INDEX(STKWp!$K$11:$K$35,IFERROR(MATCH(MIN(IF(STKWp!$D$11:$D$35&gt;AVERAGE(B523,C523),STKWp!$D$11:$D$35)),STKWp!$D$11:$D$35),1))</f>
-        <v>+II</v>
-      </c>
-      <c r="K523" s="9" t="str">
-        <f t="array" ref="K523">INDEX(BSKW!$K$11:$K$35,IFERROR(MATCH(MIN(IF(BSKW!$D$11:$D$35&gt;AVERAGE(B523,C523),BSKW!$D$11:$D$35)),BSKW!$D$11:$D$35),1))</f>
-        <v>+II</v>
-      </c>
-      <c r="L523" s="12" t="str">
-        <f t="array" ref="L523">INDEX(HTKW!$K$11:$K$36,IFERROR(MATCH(MIN(IF(HTKW!$D$11:$D$36&gt;AVERAGE(B523,C523),HTKW!$D$11:$D$36)),HTKW!$D$11:$D$36),1))</f>
-        <v>+III</v>
-      </c>
+      <c r="B523" s="8"/>
+      <c r="C523" s="9"/>
+      <c r="D523" s="23"/>
+      <c r="E523" s="23"/>
+      <c r="F523" s="9"/>
+      <c r="G523" s="9"/>
+      <c r="H523" s="9"/>
+      <c r="I523" s="9"/>
+      <c r="J523" s="9"/>
+      <c r="K523" s="9"/>
+      <c r="L523" s="12"/>
     </row>
     <row r="524" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B524" s="8"/>
@@ -25642,7 +25611,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49710E67-B736-4749-B620-06835F5DE469}">
   <dimension ref="B2:Y36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
@@ -27700,7 +27669,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DFA30DD-EAF1-4973-B290-E12CB5036732}">
   <dimension ref="B2:Y38"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
@@ -29842,7 +29811,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E4BDF32-8A22-4A66-B6B5-DB37648E7DC4}">
   <dimension ref="B2:U73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
@@ -32652,7 +32621,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4337BDE-5D5C-4814-877A-41AF49DBDF5F}">
   <dimension ref="B2:U35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A16" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
@@ -34390,7 +34359,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41A4475A-3782-4C92-8ED6-63AC240A6132}">
   <dimension ref="B2:U35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A22" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
@@ -36130,7 +36099,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51A27DBF-2298-4509-84AE-DCEFED147711}">
   <dimension ref="B2:U35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A25" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>

</xml_diff>